<commit_message>
Implemented Data Driven Test case :- Both Positive and Negative Scenarios
</commit_message>
<xml_diff>
--- a/OpenCart/testData/OpenCart LoginData.xlsx
+++ b/OpenCart/testData/OpenCart LoginData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>abc123@gmail.com</t>
+  </si>
+  <si>
+    <t>test324</t>
   </si>
 </sst>
 </file>
@@ -1063,13 +1066,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="37.2314814814815" customWidth="1"/>
     <col min="2" max="2" width="17.3055555555556" customWidth="1"/>
@@ -1140,6 +1143,15 @@
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="21" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>